<commit_message>
added Json Writer class, change jsonUtil class to universal method
</commit_message>
<xml_diff>
--- a/statistics.xlsx
+++ b/statistics.xlsx
@@ -38,25 +38,25 @@
 </t>
   </si>
   <si>
+    <t>Математика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Казанский Университет Вычислений,
+</t>
+  </si>
+  <si>
+    <t>Лингвистика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Воронежский Литературно-Переводческий Университет,
+</t>
+  </si>
+  <si>
     <t>Физика</t>
   </si>
   <si>
     <t xml:space="preserve">Московский Выдуманный Университет,
 Московский Придуманный Институт,
-</t>
-  </si>
-  <si>
-    <t>Лингвистика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Воронежский Литературно-Переводческий Университет,
-</t>
-  </si>
-  <si>
-    <t>Математика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Казанский Университет Вычислений,
 </t>
   </si>
 </sst>
@@ -153,13 +153,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>4.539999961853027</v>
+        <v>0.0</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>8</v>
@@ -187,13 +187,13 @@
         <v>11</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>0.0</v>
+        <v>4.539999961853027</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>12</v>

</xml_diff>